<commit_message>
Se desarrolla cambios en el proyecto documentacion
</commit_message>
<xml_diff>
--- a/documentacion/tablas entidades.xlsx
+++ b/documentacion/tablas entidades.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15350" windowHeight="4580" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15350" windowHeight="4580"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="73">
   <si>
     <t>Identificador de la entidad</t>
   </si>
@@ -178,6 +178,72 @@
   </si>
   <si>
     <t>id_prueba</t>
+  </si>
+  <si>
+    <t>RESPUESTAS</t>
+  </si>
+  <si>
+    <t>id_respuesta</t>
+  </si>
+  <si>
+    <t>respuesta</t>
+  </si>
+  <si>
+    <t>id_pregunta</t>
+  </si>
+  <si>
+    <t>PREGUNTAS</t>
+  </si>
+  <si>
+    <t>numero</t>
+  </si>
+  <si>
+    <t>pregunta</t>
+  </si>
+  <si>
+    <t>opcion_a</t>
+  </si>
+  <si>
+    <t>opcion_b</t>
+  </si>
+  <si>
+    <t>opcion_c</t>
+  </si>
+  <si>
+    <t>opcion_d</t>
+  </si>
+  <si>
+    <t>PRUEBA</t>
+  </si>
+  <si>
+    <t>id_empresa</t>
+  </si>
+  <si>
+    <t>fecha_inicio</t>
+  </si>
+  <si>
+    <t>fecha_final</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>cargo</t>
+  </si>
+  <si>
+    <t>EMPRESA</t>
+  </si>
+  <si>
+    <t>nit</t>
+  </si>
+  <si>
+    <t>empresa</t>
+  </si>
+  <si>
+    <t>representante</t>
+  </si>
+  <si>
+    <t>dirrecion</t>
   </si>
 </sst>
 </file>
@@ -284,21 +350,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -323,6 +374,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -606,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -617,350 +683,350 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4" t="s">
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="7"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="16"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="7"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="16"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="5" t="s">
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="7"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="16"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="7"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="16"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="7"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="16"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="7"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="16"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="7"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="16"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="7"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="16"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="7"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="16"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4" t="s">
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:C39"/>
     <mergeCell ref="A30:C30"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D31:F31"/>
@@ -969,18 +1035,18 @@
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -989,22 +1055,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I28"/>
+  <dimension ref="B1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView topLeftCell="A43" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" customWidth="1"/>
     <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2.81640625" customWidth="1"/>
     <col min="7" max="7" width="2.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.90625" customWidth="1"/>
+    <col min="9" max="9" width="42.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.35">
@@ -1013,190 +1079,190 @@
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="16"/>
+      <c r="F3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="9">
         <v>50</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="16"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="11"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="9">
         <v>50</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="16"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="9">
         <v>50</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="16"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="11"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="9">
         <v>50</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="16"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="11"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="16"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="11"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="9">
         <v>50</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="16"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="11"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="9">
         <v>50</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="16"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="11"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="16"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="11"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="9">
         <v>50</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="16"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="11"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I16" t="s">
@@ -1204,181 +1270,614 @@
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14" t="s">
+      <c r="D18" s="9"/>
+      <c r="E18" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="I18" s="16"/>
+      <c r="F18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" s="11"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="I19" s="16"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="11"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="I20" s="16"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="11"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I24" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="F25" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G25" s="13" t="s">
+      <c r="G25" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H25" s="13" t="s">
+      <c r="H25" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I25" s="13" t="s">
+      <c r="I25" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I26" s="11"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B27" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="9">
+        <v>200</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H27" s="9"/>
+      <c r="I27" s="11"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B28" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I28" s="11"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B29" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C29" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14" t="s">
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I29" s="11"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B34" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F26" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="I26" s="16"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B27" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="15" t="s">
+      <c r="F34" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I34" s="11"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B35" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="I27" s="16"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B28" s="15" t="s">
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="11"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B36" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="9">
         <v>50</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="11"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B37" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="9">
+        <v>50</v>
+      </c>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="11"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B38" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="9">
+        <v>50</v>
+      </c>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="11"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B39" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="9">
+        <v>50</v>
+      </c>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="11"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B40" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="9">
+        <v>50</v>
+      </c>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="11"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B41" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="I28" s="16"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I41" s="11"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D44" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B45" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B46" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I46" s="11"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B47" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="11"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B48" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" s="9">
+        <v>50</v>
+      </c>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="11"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B49" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" s="9">
+        <v>50</v>
+      </c>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="11"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B50" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I50" s="11"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D54" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B55" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I55" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B56" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I56" s="11"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B57" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D57" s="9">
+        <v>20</v>
+      </c>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="11"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B58" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D58" s="9">
+        <v>50</v>
+      </c>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="11"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B59" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D59" s="9">
+        <v>50</v>
+      </c>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="11"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B60" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D60" s="9">
+        <v>100</v>
+      </c>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="11"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B61" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D61" s="9">
+        <v>20</v>
+      </c>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se deesarrollan cambios den la documentacion se trata de corregir el agregar respuestas
</commit_message>
<xml_diff>
--- a/documentacion/tablas entidades.xlsx
+++ b/documentacion/tablas entidades.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15350" windowHeight="4580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15350" windowHeight="4580" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="194">
   <si>
     <t>Identificador de la entidad</t>
   </si>
@@ -244,6 +245,369 @@
   </si>
   <si>
     <t>dirrecion</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Make friends easily </t>
+  </si>
+  <si>
+    <t>Hago amigos fácilmente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Warm up quickly to others </t>
+  </si>
+  <si>
+    <t>Me intereso rápidamente por los demás</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Feel comfortable around people </t>
+  </si>
+  <si>
+    <t>Me siento a gusto estando con otras personas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Act comfortably with others </t>
+  </si>
+  <si>
+    <t>Me comporto como soy con los demás</t>
+  </si>
+  <si>
+    <t>5 Cheer people up</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Animo a los demás</t>
+  </si>
+  <si>
+    <t>6 Am hard to get to know</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Es difícil llegar a conocerme</t>
+  </si>
+  <si>
+    <t>7 Often feel uncomfortable around others</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A menudo me siento incómodo con los demás</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 Avoid contacts with others </t>
+  </si>
+  <si>
+    <t>Evito el contacto con los demás</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 Am not really interested in others </t>
+  </si>
+  <si>
+    <t>No me interesan demasiado los demás</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Keep others at a distance </t>
+  </si>
+  <si>
+    <t>Mantengo la distancia con los demás</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 Love large parties </t>
+  </si>
+  <si>
+    <t>Me encantan las fiestas grandes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 Talk to a lot of different people at parties </t>
+  </si>
+  <si>
+    <t>Hablo con mucha gente diferente en las fiestas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 Enjoy being part of a group </t>
+  </si>
+  <si>
+    <t>Disfruto de ser parte de un grupo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 Involve others in what I am doing </t>
+  </si>
+  <si>
+    <t>Involucro a los demás en lo que hago</t>
+  </si>
+  <si>
+    <t>15 Love surprise parties</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Me encantan las fiestas sorpresa</t>
+  </si>
+  <si>
+    <t>16 Prefer to be alone</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Prefiero estar solo</t>
+  </si>
+  <si>
+    <t>17 Want to be left alone</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quiero que me dejen en paz.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 Don't like crowded events </t>
+  </si>
+  <si>
+    <t>No me gustan los eventos multitudinarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 Avoid crowds </t>
+  </si>
+  <si>
+    <t>Evito las multitudes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 Seek quiet </t>
+  </si>
+  <si>
+    <t>Busco la tranquilidad.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 Take charge </t>
+  </si>
+  <si>
+    <t>Tomo el mando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 Try to lead others </t>
+  </si>
+  <si>
+    <t>Intento guiar a los demás</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 Can talk others into doing things </t>
+  </si>
+  <si>
+    <t>Puedo resultar muy convincente para que los demás hagan lo que quiero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 Seek to influence others </t>
+  </si>
+  <si>
+    <t>Trato de influenciar a los demás</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 Take control of things </t>
+  </si>
+  <si>
+    <t>Tomo el control de las cosas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 Wait for others to lead the way </t>
+  </si>
+  <si>
+    <t>Espero a que los demás lleven la delantera</t>
+  </si>
+  <si>
+    <t>27 Keep in the background</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Prefiero pasar desapercibido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 Have little to say </t>
+  </si>
+  <si>
+    <t>Tengo poco que decir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29 Don't like to draw attention to myself </t>
+  </si>
+  <si>
+    <t>No me gusta llamar la atención</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 Hold back my opinions </t>
+  </si>
+  <si>
+    <t>Me reservo mis opiniones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 Am always busy </t>
+  </si>
+  <si>
+    <t>Siempre estoy ocupado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32 Am always on the go </t>
+  </si>
+  <si>
+    <t>No paro ni un minuto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33 Do a lot in my spare time </t>
+  </si>
+  <si>
+    <t>Hago mucho en mi tiempo libre</t>
+  </si>
+  <si>
+    <t>34 Can manage many things at the same time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Puedo ocuparme de muchas cosas al mismo tiempo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35 React quickly </t>
+  </si>
+  <si>
+    <t>Reacciono rápidamente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36 Like to take it easy </t>
+  </si>
+  <si>
+    <t>Me gusta tomarme las cosas con calma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37 Like to take my time </t>
+  </si>
+  <si>
+    <t>Me gusta tomarme mi tiempo</t>
+  </si>
+  <si>
+    <t>38 Like a leisurely lifestyle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Prefiero un estilo de vida relajado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39 Let things proceed at their own pace </t>
+  </si>
+  <si>
+    <t>Dejo que las cosas sigan su propio curso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40 React slowly </t>
+  </si>
+  <si>
+    <t>Reacciono lentamente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41 Love excitement </t>
+  </si>
+  <si>
+    <t>Me encanta la adrenalina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42 Seek adventure </t>
+  </si>
+  <si>
+    <t>Busco la aventura.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43 Love action </t>
+  </si>
+  <si>
+    <t>Me encanta la acción.</t>
+  </si>
+  <si>
+    <t>44 Enjoy being part of a loud crowd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Disfruto siendo parte de un grupo muy animado de personas</t>
+  </si>
+  <si>
+    <t>45 Enjoy being reckless</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Disfruto siendo temerario</t>
+  </si>
+  <si>
+    <t>46 Act wild and crazy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Me comporto de manera desenfrenada y alocada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47 Am willing to try anything once </t>
+  </si>
+  <si>
+    <t>Estoy dispuesto a probar lo que sea por una vez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48 Seek danger </t>
+  </si>
+  <si>
+    <t>Busco el peligro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nunca haría parapente o puenting.</t>
+  </si>
+  <si>
+    <t>49 Would never go hang gliding or bungee jumping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 Dislike loud music </t>
+  </si>
+  <si>
+    <t>No me gusta la música alta</t>
+  </si>
+  <si>
+    <t>51 Radiate joy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Irradio alegría</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52 Have a lot of fun </t>
+  </si>
+  <si>
+    <t>Me divierto mucho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53 Express childlike joy </t>
+  </si>
+  <si>
+    <t>Expreso una alegría casi infantil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54 Laugh my way through life </t>
+  </si>
+  <si>
+    <t>Me tomo la vida con humor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55 Love life </t>
+  </si>
+  <si>
+    <t>Amo la vida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56 Look at the bright side of life </t>
+  </si>
+  <si>
+    <t>Miro el lado positivo de las cosas</t>
+  </si>
+  <si>
+    <t>57 Laugh aloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Me río en voz alta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58 Amuse my friends </t>
+  </si>
+  <si>
+    <t>Divierto a mis amigos</t>
+  </si>
+  <si>
+    <t>59 Am not easily amused</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> No me divierto fácilmente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60 Seldom joke around </t>
+  </si>
+  <si>
+    <t>Rara vez bromeo</t>
   </si>
 </sst>
 </file>
@@ -375,10 +739,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -672,7 +1036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:B9"/>
     </sheetView>
   </sheetViews>
@@ -852,23 +1216,23 @@
       <c r="F21" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12" t="s">
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
       <c r="D25" s="14"/>
       <c r="E25" s="15"/>
       <c r="F25" s="16"/>
@@ -956,77 +1320,77 @@
       <c r="F33" s="16"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12" t="s">
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D27:F27"/>
     <mergeCell ref="A30:C30"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D31:F31"/>
@@ -1035,18 +1399,18 @@
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="A33:C33"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="A40:C40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1055,10 +1419,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I61"/>
+  <dimension ref="B1:J61"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView topLeftCell="A52" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55:E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1066,19 +1430,20 @@
     <col min="2" max="2" width="13.1796875" customWidth="1"/>
     <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.81640625" customWidth="1"/>
-    <col min="7" max="7" width="2.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.7265625" customWidth="1"/>
+    <col min="5" max="5" width="36.81640625" customWidth="1"/>
+    <col min="6" max="6" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.81640625" customWidth="1"/>
+    <col min="8" max="8" width="2.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.35">
       <c r="D1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>21</v>
       </c>
@@ -1089,22 +1454,25 @@
         <v>43</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="10" t="s">
         <v>33</v>
       </c>
@@ -1112,19 +1480,20 @@
         <v>26</v>
       </c>
       <c r="D3" s="9"/>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="G3" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="9"/>
+      <c r="I3" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="11"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="10" t="s">
         <v>34</v>
       </c>
@@ -1138,9 +1507,10 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
-      <c r="I4" s="11"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I4" s="9"/>
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="10" t="s">
         <v>35</v>
       </c>
@@ -1154,9 +1524,10 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
-      <c r="I5" s="11"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I5" s="9"/>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="10" t="s">
         <v>36</v>
       </c>
@@ -1170,9 +1541,10 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
-      <c r="I6" s="11"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I6" s="9"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
         <v>37</v>
       </c>
@@ -1186,9 +1558,10 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
-      <c r="I7" s="11"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I7" s="9"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="10" t="s">
         <v>38</v>
       </c>
@@ -1200,9 +1573,10 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="11"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I8" s="9"/>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
         <v>39</v>
       </c>
@@ -1216,9 +1590,10 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
-      <c r="I9" s="11"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I9" s="9"/>
+      <c r="J9" s="11"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="10" t="s">
         <v>40</v>
       </c>
@@ -1232,9 +1607,10 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
-      <c r="I10" s="11"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I10" s="9"/>
+      <c r="J10" s="11"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="10" t="s">
         <v>41</v>
       </c>
@@ -1246,9 +1622,10 @@
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
-      <c r="I11" s="11"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I11" s="9"/>
+      <c r="J11" s="11"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="10" t="s">
         <v>42</v>
       </c>
@@ -1262,14 +1639,15 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
-      <c r="I12" s="11"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I16" t="s">
+      <c r="I12" s="9"/>
+      <c r="J12" s="11"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B17" s="8" t="s">
         <v>21</v>
       </c>
@@ -1280,22 +1658,25 @@
         <v>43</v>
       </c>
       <c r="E17" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="G17" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="H17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="I17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="J17" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B18" s="10" t="s">
         <v>49</v>
       </c>
@@ -1303,19 +1684,20 @@
         <v>26</v>
       </c>
       <c r="D18" s="9"/>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="9"/>
+      <c r="F18" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="G18" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9" t="s">
+      <c r="H18" s="9"/>
+      <c r="I18" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I18" s="11"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J18" s="11"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B19" s="10" t="s">
         <v>33</v>
       </c>
@@ -1324,18 +1706,19 @@
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
-      <c r="F19" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="F19" s="9"/>
       <c r="G19" s="9" t="s">
         <v>45</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="11"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" s="11"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B20" s="10" t="s">
         <v>50</v>
       </c>
@@ -1344,23 +1727,24 @@
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
-      <c r="F20" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="F20" s="9"/>
       <c r="G20" s="9" t="s">
         <v>45</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I20" s="11"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="I24" t="s">
+      <c r="I20" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J24" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B25" s="8" t="s">
         <v>21</v>
       </c>
@@ -1371,22 +1755,25 @@
         <v>43</v>
       </c>
       <c r="E25" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="G25" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="H25" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="I25" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="J25" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B26" s="10" t="s">
         <v>52</v>
       </c>
@@ -1394,19 +1781,20 @@
         <v>26</v>
       </c>
       <c r="D26" s="9"/>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="9"/>
+      <c r="F26" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="G26" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9" t="s">
+      <c r="H26" s="9"/>
+      <c r="I26" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I26" s="11"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J26" s="11"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B27" s="10" t="s">
         <v>53</v>
       </c>
@@ -1417,16 +1805,17 @@
         <v>200</v>
       </c>
       <c r="E27" s="9"/>
-      <c r="F27" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="F27" s="9"/>
       <c r="G27" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="11"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="H27" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I27" s="9"/>
+      <c r="J27" s="11"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B28" s="10" t="s">
         <v>54</v>
       </c>
@@ -1435,18 +1824,19 @@
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
-      <c r="F28" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="F28" s="9"/>
       <c r="G28" s="9" t="s">
         <v>45</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I28" s="11"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I28" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J28" s="11"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B29" s="10" t="s">
         <v>49</v>
       </c>
@@ -1455,23 +1845,24 @@
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
-      <c r="F29" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="F29" s="9"/>
       <c r="G29" s="9" t="s">
         <v>45</v>
       </c>
       <c r="H29" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I29" s="11"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I29" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J29" s="11"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
       <c r="D32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B33" s="8" t="s">
         <v>21</v>
       </c>
@@ -1482,22 +1873,25 @@
         <v>43</v>
       </c>
       <c r="E33" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="G33" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="H33" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="I33" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="J33" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B34" s="10" t="s">
         <v>54</v>
       </c>
@@ -1505,19 +1899,20 @@
         <v>26</v>
       </c>
       <c r="D34" s="9"/>
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="9"/>
+      <c r="F34" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F34" s="9" t="s">
+      <c r="G34" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9" t="s">
+      <c r="H34" s="9"/>
+      <c r="I34" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I34" s="11"/>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J34" s="11"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B35" s="10" t="s">
         <v>56</v>
       </c>
@@ -1529,9 +1924,10 @@
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
-      <c r="I35" s="11"/>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I35" s="9"/>
+      <c r="J35" s="11"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B36" s="10" t="s">
         <v>57</v>
       </c>
@@ -1545,9 +1941,10 @@
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
-      <c r="I36" s="11"/>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I36" s="9"/>
+      <c r="J36" s="11"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B37" s="10" t="s">
         <v>58</v>
       </c>
@@ -1561,9 +1958,10 @@
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
-      <c r="I37" s="11"/>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I37" s="9"/>
+      <c r="J37" s="11"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B38" s="10" t="s">
         <v>59</v>
       </c>
@@ -1577,9 +1975,10 @@
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
-      <c r="I38" s="11"/>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I38" s="9"/>
+      <c r="J38" s="11"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B39" s="10" t="s">
         <v>60</v>
       </c>
@@ -1593,9 +1992,10 @@
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
-      <c r="I39" s="11"/>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I39" s="9"/>
+      <c r="J39" s="11"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B40" s="10" t="s">
         <v>61</v>
       </c>
@@ -1609,9 +2009,10 @@
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
-      <c r="I40" s="11"/>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I40" s="9"/>
+      <c r="J40" s="11"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B41" s="10" t="s">
         <v>50</v>
       </c>
@@ -1620,23 +2021,24 @@
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
-      <c r="F41" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="F41" s="9"/>
       <c r="G41" s="9" t="s">
         <v>45</v>
       </c>
       <c r="H41" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I41" s="11"/>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I41" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J41" s="11"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.35">
       <c r="D44" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B45" s="8" t="s">
         <v>21</v>
       </c>
@@ -1647,22 +2049,25 @@
         <v>43</v>
       </c>
       <c r="E45" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F45" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F45" s="8" t="s">
+      <c r="G45" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G45" s="8" t="s">
+      <c r="H45" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H45" s="8" t="s">
+      <c r="I45" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I45" s="8" t="s">
+      <c r="J45" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B46" s="10" t="s">
         <v>54</v>
       </c>
@@ -1670,19 +2075,20 @@
         <v>26</v>
       </c>
       <c r="D46" s="9"/>
-      <c r="E46" s="9" t="s">
+      <c r="E46" s="9"/>
+      <c r="F46" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F46" s="9" t="s">
+      <c r="G46" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9" t="s">
+      <c r="H46" s="9"/>
+      <c r="I46" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I46" s="11"/>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J46" s="11"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B47" s="10" t="s">
         <v>64</v>
       </c>
@@ -1694,9 +2100,10 @@
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
-      <c r="I47" s="11"/>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I47" s="9"/>
+      <c r="J47" s="11"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B48" s="10" t="s">
         <v>65</v>
       </c>
@@ -1710,9 +2117,10 @@
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
       <c r="H48" s="9"/>
-      <c r="I48" s="11"/>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I48" s="9"/>
+      <c r="J48" s="11"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B49" s="10" t="s">
         <v>67</v>
       </c>
@@ -1726,9 +2134,10 @@
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
       <c r="H49" s="9"/>
-      <c r="I49" s="11"/>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I49" s="9"/>
+      <c r="J49" s="11"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B50" s="10" t="s">
         <v>63</v>
       </c>
@@ -1737,23 +2146,24 @@
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
-      <c r="F50" s="9" t="s">
-        <v>27</v>
-      </c>
+      <c r="F50" s="9"/>
       <c r="G50" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H50" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I50" s="11"/>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I50" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J50" s="11"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.35">
       <c r="D54" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B55" s="8" t="s">
         <v>21</v>
       </c>
@@ -1764,22 +2174,25 @@
         <v>43</v>
       </c>
       <c r="E55" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F55" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F55" s="8" t="s">
+      <c r="G55" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G55" s="8" t="s">
+      <c r="H55" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H55" s="8" t="s">
+      <c r="I55" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I55" s="8" t="s">
+      <c r="J55" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B56" s="10" t="s">
         <v>63</v>
       </c>
@@ -1787,19 +2200,20 @@
         <v>26</v>
       </c>
       <c r="D56" s="9"/>
-      <c r="E56" s="9" t="s">
+      <c r="E56" s="9"/>
+      <c r="F56" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F56" s="9" t="s">
+      <c r="G56" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9" t="s">
+      <c r="H56" s="9"/>
+      <c r="I56" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I56" s="11"/>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J56" s="11"/>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B57" s="10" t="s">
         <v>69</v>
       </c>
@@ -1813,9 +2227,10 @@
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
-      <c r="I57" s="11"/>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I57" s="9"/>
+      <c r="J57" s="11"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B58" s="10" t="s">
         <v>70</v>
       </c>
@@ -1829,9 +2244,10 @@
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
-      <c r="I58" s="11"/>
-    </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I58" s="9"/>
+      <c r="J58" s="11"/>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B59" s="10" t="s">
         <v>71</v>
       </c>
@@ -1845,9 +2261,10 @@
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
       <c r="H59" s="9"/>
-      <c r="I59" s="11"/>
-    </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I59" s="9"/>
+      <c r="J59" s="11"/>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B60" s="10" t="s">
         <v>72</v>
       </c>
@@ -1861,9 +2278,10 @@
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
       <c r="H60" s="9"/>
-      <c r="I60" s="11"/>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I60" s="9"/>
+      <c r="J60" s="11"/>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B61" s="10" t="s">
         <v>37</v>
       </c>
@@ -1877,10 +2295,512 @@
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
-      <c r="I61" s="11"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="77.6328125" customWidth="1"/>
+    <col min="2" max="2" width="74.453125" customWidth="1"/>
+    <col min="3" max="3" width="82.6328125" customWidth="1"/>
+    <col min="4" max="4" width="10.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>132</v>
+      </c>
+      <c r="B30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>138</v>
+      </c>
+      <c r="B33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>140</v>
+      </c>
+      <c r="B34" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>142</v>
+      </c>
+      <c r="B35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>144</v>
+      </c>
+      <c r="B36" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>146</v>
+      </c>
+      <c r="B37" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>148</v>
+      </c>
+      <c r="B38" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>150</v>
+      </c>
+      <c r="B39" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>152</v>
+      </c>
+      <c r="B40" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>156</v>
+      </c>
+      <c r="B42" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>158</v>
+      </c>
+      <c r="B43" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>160</v>
+      </c>
+      <c r="B44" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>164</v>
+      </c>
+      <c r="B46" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>166</v>
+      </c>
+      <c r="B47" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>168</v>
+      </c>
+      <c r="B48" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>171</v>
+      </c>
+      <c r="B49" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>172</v>
+      </c>
+      <c r="B50" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>174</v>
+      </c>
+      <c r="B51" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>176</v>
+      </c>
+      <c r="B52" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>178</v>
+      </c>
+      <c r="B53" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>180</v>
+      </c>
+      <c r="B54" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>182</v>
+      </c>
+      <c r="B55" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>184</v>
+      </c>
+      <c r="B56" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>186</v>
+      </c>
+      <c r="B57" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>188</v>
+      </c>
+      <c r="B58" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>190</v>
+      </c>
+      <c r="B59" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>192</v>
+      </c>
+      <c r="B60" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se corregio algunos detalles de las tablas, y se trata de corregir op3
</commit_message>
<xml_diff>
--- a/documentacion/tablas entidades.xlsx
+++ b/documentacion/tablas entidades.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="341">
   <si>
     <t>Identificador de la entidad</t>
   </si>
@@ -250,364 +251,805 @@
     <t>Descripcion</t>
   </si>
   <si>
-    <t xml:space="preserve">1 Make friends easily </t>
-  </si>
-  <si>
     <t>Hago amigos fácilmente</t>
   </si>
   <si>
-    <t xml:space="preserve">2 Warm up quickly to others </t>
-  </si>
-  <si>
     <t>Me intereso rápidamente por los demás</t>
   </si>
   <si>
-    <t xml:space="preserve">3 Feel comfortable around people </t>
-  </si>
-  <si>
     <t>Me siento a gusto estando con otras personas</t>
   </si>
   <si>
-    <t xml:space="preserve">4 Act comfortably with others </t>
-  </si>
-  <si>
     <t>Me comporto como soy con los demás</t>
   </si>
   <si>
-    <t>5 Cheer people up</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Animo a los demás</t>
-  </si>
-  <si>
-    <t>6 Am hard to get to know</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Es difícil llegar a conocerme</t>
   </si>
   <si>
-    <t>7 Often feel uncomfortable around others</t>
-  </si>
-  <si>
     <t xml:space="preserve"> A menudo me siento incómodo con los demás</t>
   </si>
   <si>
-    <t xml:space="preserve">8 Avoid contacts with others </t>
-  </si>
-  <si>
     <t>Evito el contacto con los demás</t>
   </si>
   <si>
-    <t xml:space="preserve">9 Am not really interested in others </t>
-  </si>
-  <si>
     <t>No me interesan demasiado los demás</t>
   </si>
   <si>
-    <t xml:space="preserve">10 Keep others at a distance </t>
-  </si>
-  <si>
     <t>Mantengo la distancia con los demás</t>
   </si>
   <si>
-    <t xml:space="preserve">11 Love large parties </t>
-  </si>
-  <si>
     <t>Me encantan las fiestas grandes</t>
   </si>
   <si>
-    <t xml:space="preserve">12 Talk to a lot of different people at parties </t>
-  </si>
-  <si>
     <t>Hablo con mucha gente diferente en las fiestas</t>
   </si>
   <si>
-    <t xml:space="preserve">13 Enjoy being part of a group </t>
-  </si>
-  <si>
     <t>Disfruto de ser parte de un grupo</t>
   </si>
   <si>
-    <t xml:space="preserve">14 Involve others in what I am doing </t>
-  </si>
-  <si>
     <t>Involucro a los demás en lo que hago</t>
   </si>
   <si>
-    <t>15 Love surprise parties</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Me encantan las fiestas sorpresa</t>
   </si>
   <si>
-    <t>16 Prefer to be alone</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Prefiero estar solo</t>
   </si>
   <si>
-    <t>17 Want to be left alone</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Quiero que me dejen en paz.</t>
   </si>
   <si>
-    <t xml:space="preserve">18 Don't like crowded events </t>
-  </si>
-  <si>
     <t>No me gustan los eventos multitudinarios</t>
   </si>
   <si>
-    <t xml:space="preserve">19 Avoid crowds </t>
-  </si>
-  <si>
     <t>Evito las multitudes.</t>
   </si>
   <si>
-    <t xml:space="preserve">20 Seek quiet </t>
-  </si>
-  <si>
     <t>Busco la tranquilidad.</t>
   </si>
   <si>
-    <t xml:space="preserve">21 Take charge </t>
-  </si>
-  <si>
     <t>Tomo el mando</t>
   </si>
   <si>
-    <t xml:space="preserve">22 Try to lead others </t>
-  </si>
-  <si>
     <t>Intento guiar a los demás</t>
   </si>
   <si>
-    <t xml:space="preserve">23 Can talk others into doing things </t>
-  </si>
-  <si>
     <t>Puedo resultar muy convincente para que los demás hagan lo que quiero</t>
   </si>
   <si>
-    <t xml:space="preserve">24 Seek to influence others </t>
-  </si>
-  <si>
     <t>Trato de influenciar a los demás</t>
   </si>
   <si>
-    <t xml:space="preserve">25 Take control of things </t>
-  </si>
-  <si>
     <t>Tomo el control de las cosas</t>
   </si>
   <si>
-    <t xml:space="preserve">26 Wait for others to lead the way </t>
-  </si>
-  <si>
     <t>Espero a que los demás lleven la delantera</t>
   </si>
   <si>
-    <t>27 Keep in the background</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Prefiero pasar desapercibido</t>
   </si>
   <si>
-    <t xml:space="preserve">28 Have little to say </t>
-  </si>
-  <si>
     <t>Tengo poco que decir</t>
   </si>
   <si>
-    <t xml:space="preserve">29 Don't like to draw attention to myself </t>
-  </si>
-  <si>
     <t>No me gusta llamar la atención</t>
   </si>
   <si>
-    <t xml:space="preserve">30 Hold back my opinions </t>
-  </si>
-  <si>
     <t>Me reservo mis opiniones</t>
   </si>
   <si>
-    <t xml:space="preserve">31 Am always busy </t>
-  </si>
-  <si>
     <t>Siempre estoy ocupado</t>
   </si>
   <si>
-    <t xml:space="preserve">32 Am always on the go </t>
-  </si>
-  <si>
     <t>No paro ni un minuto</t>
   </si>
   <si>
-    <t xml:space="preserve">33 Do a lot in my spare time </t>
-  </si>
-  <si>
     <t>Hago mucho en mi tiempo libre</t>
   </si>
   <si>
-    <t>34 Can manage many things at the same time</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Puedo ocuparme de muchas cosas al mismo tiempo</t>
   </si>
   <si>
-    <t xml:space="preserve">35 React quickly </t>
-  </si>
-  <si>
     <t>Reacciono rápidamente</t>
   </si>
   <si>
-    <t xml:space="preserve">36 Like to take it easy </t>
-  </si>
-  <si>
     <t>Me gusta tomarme las cosas con calma</t>
   </si>
   <si>
-    <t xml:space="preserve">37 Like to take my time </t>
-  </si>
-  <si>
     <t>Me gusta tomarme mi tiempo</t>
   </si>
   <si>
-    <t>38 Like a leisurely lifestyle</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Prefiero un estilo de vida relajado</t>
   </si>
   <si>
-    <t xml:space="preserve">39 Let things proceed at their own pace </t>
-  </si>
-  <si>
     <t>Dejo que las cosas sigan su propio curso</t>
   </si>
   <si>
-    <t xml:space="preserve">40 React slowly </t>
-  </si>
-  <si>
     <t>Reacciono lentamente</t>
   </si>
   <si>
-    <t xml:space="preserve">41 Love excitement </t>
-  </si>
-  <si>
     <t>Me encanta la adrenalina</t>
   </si>
   <si>
-    <t xml:space="preserve">42 Seek adventure </t>
-  </si>
-  <si>
     <t>Busco la aventura.</t>
   </si>
   <si>
-    <t xml:space="preserve">43 Love action </t>
-  </si>
-  <si>
     <t>Me encanta la acción.</t>
   </si>
   <si>
-    <t>44 Enjoy being part of a loud crowd</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Disfruto siendo parte de un grupo muy animado de personas</t>
   </si>
   <si>
-    <t>45 Enjoy being reckless</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Disfruto siendo temerario</t>
   </si>
   <si>
-    <t>46 Act wild and crazy</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Me comporto de manera desenfrenada y alocada</t>
   </si>
   <si>
-    <t xml:space="preserve">47 Am willing to try anything once </t>
-  </si>
-  <si>
     <t>Estoy dispuesto a probar lo que sea por una vez</t>
   </si>
   <si>
-    <t xml:space="preserve">48 Seek danger </t>
-  </si>
-  <si>
     <t>Busco el peligro</t>
   </si>
   <si>
     <t xml:space="preserve"> Nunca haría parapente o puenting.</t>
   </si>
   <si>
-    <t>49 Would never go hang gliding or bungee jumping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50 Dislike loud music </t>
-  </si>
-  <si>
     <t>No me gusta la música alta</t>
   </si>
   <si>
-    <t>51 Radiate joy</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Irradio alegría</t>
   </si>
   <si>
-    <t xml:space="preserve">52 Have a lot of fun </t>
-  </si>
-  <si>
     <t>Me divierto mucho</t>
   </si>
   <si>
-    <t xml:space="preserve">53 Express childlike joy </t>
-  </si>
-  <si>
     <t>Expreso una alegría casi infantil</t>
   </si>
   <si>
-    <t xml:space="preserve">54 Laugh my way through life </t>
-  </si>
-  <si>
     <t>Me tomo la vida con humor</t>
   </si>
   <si>
-    <t xml:space="preserve">55 Love life </t>
-  </si>
-  <si>
     <t>Amo la vida</t>
   </si>
   <si>
-    <t xml:space="preserve">56 Look at the bright side of life </t>
-  </si>
-  <si>
     <t>Miro el lado positivo de las cosas</t>
   </si>
   <si>
-    <t>57 Laugh aloud</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Me río en voz alta</t>
   </si>
   <si>
-    <t xml:space="preserve">58 Amuse my friends </t>
-  </si>
-  <si>
     <t>Divierto a mis amigos</t>
   </si>
   <si>
-    <t>59 Am not easily amused</t>
-  </si>
-  <si>
     <t xml:space="preserve"> No me divierto fácilmente</t>
   </si>
   <si>
-    <t xml:space="preserve">60 Seldom joke around </t>
-  </si>
-  <si>
     <t>Rara vez bromeo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make friends easily </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warm up quickly to others </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feel comfortable around people </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Act comfortably with others </t>
+  </si>
+  <si>
+    <t>Cheer people up</t>
+  </si>
+  <si>
+    <t>Am hard to get to know</t>
+  </si>
+  <si>
+    <t>Often feel uncomfortable around others</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avoid contacts with others </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Am not really interested in others </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep others at a distance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Love large parties </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talk to a lot of different people at parties </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enjoy being part of a group </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Involve others in what I am doing </t>
+  </si>
+  <si>
+    <t>Love surprise parties</t>
+  </si>
+  <si>
+    <t>Prefer to be alone</t>
+  </si>
+  <si>
+    <t>Want to be left alone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't like crowded events </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avoid crowds </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seek quiet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take charge </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to lead others </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can talk others into doing things </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seek to influence others </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take control of things </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wait for others to lead the way </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have little to say </t>
+  </si>
+  <si>
+    <t>Keep in the background</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't like to draw attention to myself </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hold back my opinions </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Am always busy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Am always on the go </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do a lot in my spare time </t>
+  </si>
+  <si>
+    <t>Can manage many things at the same time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seldom joke around </t>
+  </si>
+  <si>
+    <t>Am not easily amused</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amuse my friends </t>
+  </si>
+  <si>
+    <t>Laugh aloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Look at the bright side of life </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Love life </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laugh my way through life </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Express childlike joy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have a lot of fun </t>
+  </si>
+  <si>
+    <t>Radiate joy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dislike loud music </t>
+  </si>
+  <si>
+    <t>Would never go hang gliding or bungee jumping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seek danger </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Am willing to try anything once </t>
+  </si>
+  <si>
+    <t>Act wild and crazy</t>
+  </si>
+  <si>
+    <t>Enjoy being reckless</t>
+  </si>
+  <si>
+    <t>Enjoy being part of a loud crowd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Love action </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seek adventure </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Love excitement </t>
+  </si>
+  <si>
+    <t xml:space="preserve">React slowly </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let things proceed at their own pace </t>
+  </si>
+  <si>
+    <t>Like a leisurely lifestyle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Like to take my time </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Like to take it easy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">React quickly </t>
+  </si>
+  <si>
+    <t>Animar a la gente</t>
+  </si>
+  <si>
+    <t>Buenos días.</t>
+  </si>
+  <si>
+    <t>Buenas tardes.</t>
+  </si>
+  <si>
+    <t>Buenas noches.</t>
+  </si>
+  <si>
+    <t>Hasta luego.</t>
+  </si>
+  <si>
+    <t>Hasta mañana.</t>
+  </si>
+  <si>
+    <t>Gracias.</t>
+  </si>
+  <si>
+    <t>De nada</t>
+  </si>
+  <si>
+    <t>Quiero presentarte a mi novio</t>
+  </si>
+  <si>
+    <t>Mucho gusto.</t>
+  </si>
+  <si>
+    <t>¿Cómo te va?</t>
+  </si>
+  <si>
+    <t>Muy bien.</t>
+  </si>
+  <si>
+    <t>Todo bien.</t>
+  </si>
+  <si>
+    <t>Todo legal.</t>
+  </si>
+  <si>
+    <t>¿Qué hay de nuevo?</t>
+  </si>
+  <si>
+    <t>Nada, todo igual.</t>
+  </si>
+  <si>
+    <t>¿Hablas portugués?</t>
+  </si>
+  <si>
+    <t>¿A qué hora nos encontramos?</t>
+  </si>
+  <si>
+    <t>A las cinco de la tarde.</t>
+  </si>
+  <si>
+    <t>Ok, de acuerdo.</t>
+  </si>
+  <si>
+    <t>¿Cómo te llamas?</t>
+  </si>
+  <si>
+    <t>¿De dónde eres?</t>
+  </si>
+  <si>
+    <t>Soy de Argentina, estoy aquí tomando unas vacaciones.</t>
+  </si>
+  <si>
+    <t>¿Estás solo?</t>
+  </si>
+  <si>
+    <t>¿Estás casado?</t>
+  </si>
+  <si>
+    <t>Te quiero mucho/Me gustas mucho.</t>
+  </si>
+  <si>
+    <t>Te gusta bailar?</t>
+  </si>
+  <si>
+    <t>¿Nos vamos?</t>
+  </si>
+  <si>
+    <t>Quiero ir al shopping a comprar ropa.</t>
+  </si>
+  <si>
+    <t>¿Cuánto es?</t>
+  </si>
+  <si>
+    <t>¿Puedo pagar con tarjeta de crédito?</t>
+  </si>
+  <si>
+    <t>No, solo al contado.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el precio?</t>
+  </si>
+  <si>
+    <t>Pero ese precio está equivocado.</t>
+  </si>
+  <si>
+    <t>¿Puedo hablar con el responsable?</t>
+  </si>
+  <si>
+    <t>No, ahora él no está.</t>
+  </si>
+  <si>
+    <t>Bueno, vámonos.</t>
+  </si>
+  <si>
+    <t>¿Tienes hambre?</t>
+  </si>
+  <si>
+    <t>Sí, tengo mucha hambre.</t>
+  </si>
+  <si>
+    <t>¿Quieres almorzar en un restaurante cerca de aquí?</t>
+  </si>
+  <si>
+    <t>¡Vamos!</t>
+  </si>
+  <si>
+    <t>¿Tendrá estacionamiento?</t>
+  </si>
+  <si>
+    <t>Creo que sí.</t>
+  </si>
+  <si>
+    <t>También podemos ir en taxi.</t>
+  </si>
+  <si>
+    <t>Pero yo prefiero ir con el auto.</t>
+  </si>
+  <si>
+    <t>OK, vamos con el auto.</t>
+  </si>
+  <si>
+    <t>Quiero un vaso de agua/vino/gaseosa</t>
+  </si>
+  <si>
+    <t>Quiero jugo de naranja/ananá/durazno</t>
+  </si>
+  <si>
+    <t>No tengo tenedor/cuchillo/cuchara/plato.</t>
+  </si>
+  <si>
+    <t>¿Qué me recomienda?</t>
+  </si>
+  <si>
+    <t>¿Puede traerme la carta/el menú+B95?</t>
+  </si>
+  <si>
+    <t>¿Haces traducciones de portugués?</t>
+  </si>
+  <si>
+    <t>¿Eres traductora de portugués?</t>
+  </si>
+  <si>
+    <t>¿Quieres tomar un café o prefieres un té?</t>
+  </si>
+  <si>
+    <t>Prefiero un café.</t>
+  </si>
+  <si>
+    <t>¿Hoy hay after office (happy hour)?</t>
+  </si>
+  <si>
+    <t>¿Vamos a tomar un chop?</t>
+  </si>
+  <si>
+    <t>¿Lloverá mañana?</t>
+  </si>
+  <si>
+    <t>¡Dios! No me gusta la lluvia.</t>
+  </si>
+  <si>
+    <t>Me gusta el sol.</t>
+  </si>
+  <si>
+    <t>¿Mañana tienes una reunión en la oficina?</t>
+  </si>
+  <si>
+    <t>Sí, a las 8 de la mañana, tenemos una cita con el traductor de portugués.</t>
+  </si>
+  <si>
+    <t>No te olvides de llevar tu carpeta con los papeles del proyecto.</t>
+  </si>
+  <si>
+    <t>No, no me voy a olvidar.</t>
+  </si>
+  <si>
+    <t>¿El traductor se queda mucho tiempo en Brasil?</t>
+  </si>
+  <si>
+    <t>No, solo dos días.</t>
+  </si>
+  <si>
+    <t>Se va el viernes.</t>
+  </si>
+  <si>
+    <t>¿Cómo se dice domingo en portugués?</t>
+  </si>
+  <si>
+    <t>¿Cómo se pronuncia esa palabra?</t>
+  </si>
+  <si>
+    <t>¿Estás listo?</t>
+  </si>
+  <si>
+    <t>Eso no me gusta.</t>
+  </si>
+  <si>
+    <t>¿Dónde está el baño?</t>
+  </si>
+  <si>
+    <t>Tengo clase de portugués.</t>
+  </si>
+  <si>
+    <t>Hoy estoy disponible.</t>
+  </si>
+  <si>
+    <t>Manejas muy rápido.</t>
+  </si>
+  <si>
+    <t>Estoy enojado.</t>
+  </si>
+  <si>
+    <t>Estoy molesto.</t>
+  </si>
+  <si>
+    <t>Estoy cansado.</t>
+  </si>
+  <si>
+    <t>Estoy contento.</t>
+  </si>
+  <si>
+    <t>Tengo miedo.</t>
+  </si>
+  <si>
+    <t>Compré dos entradas para el recital/show de Chico.</t>
+  </si>
+  <si>
+    <t>Me siento mal, estoy enfermo.</t>
+  </si>
+  <si>
+    <t>¿Puede sacar una fotografia?</t>
+  </si>
+  <si>
+    <t>¿Le gustaría visitar la catedral?</t>
+  </si>
+  <si>
+    <t>¿A qué hora comienza el show?</t>
+  </si>
+  <si>
+    <t>¿La parada de autobús queda lejos?</t>
+  </si>
+  <si>
+    <t>Me gustaría alquilar un coche.</t>
+  </si>
+  <si>
+    <t>¿Ya visitaste el Pan de Açúcar?</t>
+  </si>
+  <si>
+    <t>Tener vista de lince</t>
+  </si>
+  <si>
+    <t>Tener muy buena vista</t>
+  </si>
+  <si>
+    <t>Ser un gallina</t>
+  </si>
+  <si>
+    <t>Ser un cobarde</t>
+  </si>
+  <si>
+    <t>Estar en la edad del pavo</t>
+  </si>
+  <si>
+    <t>Estar en la adolescencia</t>
+  </si>
+  <si>
+    <t>Ser la oveja negra</t>
+  </si>
+  <si>
+    <t>Ser un descarriado, ser el que no tiene éxito</t>
+  </si>
+  <si>
+    <t>Estar como una cabra</t>
+  </si>
+  <si>
+    <t>Estar loco</t>
+  </si>
+  <si>
+    <t>No ver tres en un burro</t>
+  </si>
+  <si>
+    <t>Tener muy mala vista</t>
+  </si>
+  <si>
+    <t>Dar gato por liebre</t>
+  </si>
+  <si>
+    <t>Engañar, timar</t>
+  </si>
+  <si>
+    <t>Ser un rata</t>
+  </si>
+  <si>
+    <t>Ser muy tacaño</t>
+  </si>
+  <si>
+    <t>Verle las orejas al lobo</t>
+  </si>
+  <si>
+    <t>Darse cuenta de un peligro</t>
+  </si>
+  <si>
+    <t>Tener memoria de pez</t>
+  </si>
+  <si>
+    <t>Tener muy mala memoria</t>
+  </si>
+  <si>
+    <t>Lavarse las manos</t>
+  </si>
+  <si>
+    <t>Eludir una responsabilidad</t>
+  </si>
+  <si>
+    <t>Hacer algo al pie de la letra</t>
+  </si>
+  <si>
+    <t>Hacer algo según las instrucciones</t>
+  </si>
+  <si>
+    <t>No tener ni pies ni cabeza</t>
+  </si>
+  <si>
+    <t>No tener sentido</t>
+  </si>
+  <si>
+    <t>Meter la pata</t>
+  </si>
+  <si>
+    <t>Cometer un error</t>
+  </si>
+  <si>
+    <t>No pegar ojo</t>
+  </si>
+  <si>
+    <t>Pasar la noche sin dormir</t>
+  </si>
+  <si>
+    <t>Sin pelos en la lengua</t>
+  </si>
+  <si>
+    <t>Honesto, sincere</t>
+  </si>
+  <si>
+    <t>Estar hasta las narices</t>
+  </si>
+  <si>
+    <t>Estar harto</t>
+  </si>
+  <si>
+    <t>Dormir a pierna suelta</t>
+  </si>
+  <si>
+    <t>Dormir profundamente</t>
+  </si>
+  <si>
+    <t>Buscar tres pies al gato</t>
+  </si>
+  <si>
+    <t>Hacer algo más complicado de lo que es</t>
+  </si>
+  <si>
+    <t>Andar con pies de plomo</t>
+  </si>
+  <si>
+    <t>Actuar con cautela</t>
+  </si>
+  <si>
+    <t>No haber color</t>
+  </si>
+  <si>
+    <t>No se puede comparar</t>
+  </si>
+  <si>
+    <t>Tener la negra</t>
+  </si>
+  <si>
+    <t>Tener mala suerte</t>
+  </si>
+  <si>
+    <t>Dar en el blanco</t>
+  </si>
+  <si>
+    <t>Acertar</t>
+  </si>
+  <si>
+    <t>Verlo todo de color de rosa</t>
+  </si>
+  <si>
+    <t>Ser demasiado optimista</t>
+  </si>
+  <si>
+    <t>Buscar el príncipe azul</t>
+  </si>
+  <si>
+    <t>Buscar al hombre ideal</t>
+  </si>
+  <si>
+    <t>Ponerse morado</t>
+  </si>
+  <si>
+    <t>Comer demasiado</t>
+  </si>
+  <si>
+    <t>Estar sin blanca</t>
+  </si>
+  <si>
+    <t>No tener dinero</t>
+  </si>
+  <si>
+    <t>Poner verde a alguien</t>
+  </si>
+  <si>
+    <t>Criticar a alguien</t>
+  </si>
+  <si>
+    <t>Tener sangre azul</t>
+  </si>
+  <si>
+    <t>Ser de la realeza o de buena familia</t>
+  </si>
+  <si>
+    <t>Encontrar tu media naranja</t>
+  </si>
+  <si>
+    <t>Conocer a tu pareja ideal</t>
   </si>
 </sst>
 </file>
@@ -739,10 +1181,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1216,23 +1658,23 @@
       <c r="F21" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13" t="s">
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
       <c r="D25" s="14"/>
       <c r="E25" s="15"/>
       <c r="F25" s="16"/>
@@ -1320,77 +1762,77 @@
       <c r="F33" s="16"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13" t="s">
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="12" t="s">
+      <c r="A37" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:C39"/>
     <mergeCell ref="A30:C30"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D31:F31"/>
@@ -1399,18 +1841,18 @@
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2306,501 +2748,3034 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+      <selection activeCell="F60" sqref="C1:F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="77.6328125" customWidth="1"/>
-    <col min="2" max="2" width="74.453125" customWidth="1"/>
-    <col min="3" max="3" width="82.6328125" customWidth="1"/>
-    <col min="4" max="4" width="10.90625" customWidth="1"/>
+    <col min="2" max="2" width="43.1796875" customWidth="1"/>
+    <col min="3" max="3" width="58.54296875" customWidth="1"/>
+    <col min="4" max="4" width="49.7265625" customWidth="1"/>
+    <col min="5" max="5" width="44.54296875" customWidth="1"/>
+    <col min="6" max="6" width="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" t="s">
         <v>74</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="E2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E3" t="s">
         <v>76</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D4" t="s">
+        <v>217</v>
+      </c>
+      <c r="E4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D5" t="s">
+        <v>296</v>
+      </c>
+      <c r="E5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D6" t="s">
         <v>78</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E6" t="s">
+        <v>251</v>
+      </c>
+      <c r="F6" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D7" t="s">
+        <v>310</v>
+      </c>
+      <c r="E7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="F7" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" t="s">
+        <v>319</v>
+      </c>
+      <c r="D8" t="s">
+        <v>273</v>
+      </c>
+      <c r="E8" t="s">
+        <v>250</v>
+      </c>
+      <c r="F8" t="s">
         <v>80</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" t="s">
+        <v>206</v>
+      </c>
+      <c r="D9" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="E9" t="s">
+        <v>275</v>
+      </c>
+      <c r="F9" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" t="s">
+        <v>215</v>
+      </c>
+      <c r="E10" t="s">
         <v>82</v>
       </c>
-      <c r="B5" t="s">
+      <c r="F10" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" t="s">
+        <v>268</v>
+      </c>
+      <c r="D11" t="s">
+        <v>313</v>
+      </c>
+      <c r="E11" t="s">
+        <v>248</v>
+      </c>
+      <c r="F11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" t="s">
         <v>84</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D12" t="s">
+        <v>220</v>
+      </c>
+      <c r="E12" t="s">
+        <v>229</v>
+      </c>
+      <c r="F12" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" t="s">
+        <v>279</v>
+      </c>
+      <c r="D13" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="E13" t="s">
+        <v>334</v>
+      </c>
+      <c r="F13" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D14" t="s">
+        <v>219</v>
+      </c>
+      <c r="E14" t="s">
         <v>86</v>
       </c>
-      <c r="B7" t="s">
+      <c r="F14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" t="s">
+        <v>243</v>
+      </c>
+      <c r="D15" t="s">
+        <v>291</v>
+      </c>
+      <c r="E15" t="s">
+        <v>233</v>
+      </c>
+      <c r="F15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" t="s">
         <v>88</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D16" t="s">
+        <v>285</v>
+      </c>
+      <c r="E16" t="s">
+        <v>241</v>
+      </c>
+      <c r="F16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" t="s">
+        <v>256</v>
+      </c>
+      <c r="D17" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="E17" t="s">
+        <v>282</v>
+      </c>
+      <c r="F17" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" t="s">
+        <v>282</v>
+      </c>
+      <c r="D18" t="s">
+        <v>249</v>
+      </c>
+      <c r="E18" t="s">
         <v>90</v>
       </c>
-      <c r="B9" t="s">
+      <c r="F18" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19" t="s">
+        <v>283</v>
+      </c>
+      <c r="D19" t="s">
+        <v>304</v>
+      </c>
+      <c r="E19" t="s">
+        <v>216</v>
+      </c>
+      <c r="F19" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" t="s">
         <v>92</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D20" t="s">
+        <v>288</v>
+      </c>
+      <c r="E20" t="s">
+        <v>262</v>
+      </c>
+      <c r="F20" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" t="s">
+        <v>310</v>
+      </c>
+      <c r="D21" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="E21" t="s">
+        <v>310</v>
+      </c>
+      <c r="F21" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C22" t="s">
+        <v>222</v>
+      </c>
+      <c r="D22" t="s">
+        <v>216</v>
+      </c>
+      <c r="E22" t="s">
         <v>94</v>
       </c>
-      <c r="B11" t="s">
+      <c r="F22" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" t="s">
+        <v>210</v>
+      </c>
+      <c r="D23" t="s">
+        <v>323</v>
+      </c>
+      <c r="E23" t="s">
+        <v>263</v>
+      </c>
+      <c r="F23" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>156</v>
+      </c>
+      <c r="C24" t="s">
         <v>96</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D24" t="s">
+        <v>305</v>
+      </c>
+      <c r="E24" t="s">
+        <v>318</v>
+      </c>
+      <c r="F24" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" t="s">
+        <v>222</v>
+      </c>
+      <c r="D25" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="E25" t="s">
+        <v>258</v>
+      </c>
+      <c r="F25" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>158</v>
+      </c>
+      <c r="C26" t="s">
+        <v>330</v>
+      </c>
+      <c r="D26" t="s">
+        <v>264</v>
+      </c>
+      <c r="E26" t="s">
         <v>98</v>
       </c>
-      <c r="B13" t="s">
+      <c r="F26" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>160</v>
+      </c>
+      <c r="C27" t="s">
+        <v>297</v>
+      </c>
+      <c r="D27" t="s">
+        <v>333</v>
+      </c>
+      <c r="E27" t="s">
+        <v>308</v>
+      </c>
+      <c r="F27" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>159</v>
+      </c>
+      <c r="C28" t="s">
         <v>100</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D28" t="s">
+        <v>312</v>
+      </c>
+      <c r="E28" t="s">
+        <v>211</v>
+      </c>
+      <c r="F28" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>161</v>
+      </c>
+      <c r="C29" t="s">
+        <v>201</v>
+      </c>
+      <c r="D29" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="E29" t="s">
+        <v>204</v>
+      </c>
+      <c r="F29" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>162</v>
+      </c>
+      <c r="C30" t="s">
+        <v>215</v>
+      </c>
+      <c r="D30" t="s">
+        <v>285</v>
+      </c>
+      <c r="E30" t="s">
         <v>102</v>
       </c>
-      <c r="B15" t="s">
+      <c r="F30" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>163</v>
+      </c>
+      <c r="C31" t="s">
+        <v>247</v>
+      </c>
+      <c r="D31" t="s">
+        <v>314</v>
+      </c>
+      <c r="E31" t="s">
+        <v>234</v>
+      </c>
+      <c r="F31" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>164</v>
+      </c>
+      <c r="C32" t="s">
         <v>104</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D32" t="s">
+        <v>265</v>
+      </c>
+      <c r="E32" t="s">
+        <v>293</v>
+      </c>
+      <c r="F32" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>165</v>
+      </c>
+      <c r="C33" t="s">
+        <v>292</v>
+      </c>
+      <c r="D33" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="E33" t="s">
+        <v>236</v>
+      </c>
+      <c r="F33" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>166</v>
+      </c>
+      <c r="C34" t="s">
+        <v>264</v>
+      </c>
+      <c r="D34" t="s">
+        <v>216</v>
+      </c>
+      <c r="E34" t="s">
         <v>106</v>
       </c>
-      <c r="B17" t="s">
+      <c r="F34" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>192</v>
+      </c>
+      <c r="C35" t="s">
+        <v>224</v>
+      </c>
+      <c r="D35" t="s">
+        <v>283</v>
+      </c>
+      <c r="E35" t="s">
+        <v>263</v>
+      </c>
+      <c r="F35" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>191</v>
+      </c>
+      <c r="C36" t="s">
         <v>108</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D36" t="s">
+        <v>292</v>
+      </c>
+      <c r="E36" t="s">
+        <v>311</v>
+      </c>
+      <c r="F36" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>190</v>
+      </c>
+      <c r="C37" t="s">
+        <v>250</v>
+      </c>
+      <c r="D37" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="E37" t="s">
+        <v>328</v>
+      </c>
+      <c r="F37" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>189</v>
+      </c>
+      <c r="C38" t="s">
+        <v>320</v>
+      </c>
+      <c r="D38" t="s">
+        <v>277</v>
+      </c>
+      <c r="E38" t="s">
         <v>110</v>
       </c>
-      <c r="B19" t="s">
+      <c r="F38" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>188</v>
+      </c>
+      <c r="C39" t="s">
+        <v>290</v>
+      </c>
+      <c r="D39" t="s">
+        <v>316</v>
+      </c>
+      <c r="E39" t="s">
+        <v>302</v>
+      </c>
+      <c r="F39" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>187</v>
+      </c>
+      <c r="C40" t="s">
         <v>112</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D40" t="s">
+        <v>289</v>
+      </c>
+      <c r="E40" t="s">
+        <v>328</v>
+      </c>
+      <c r="F40" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>186</v>
+      </c>
+      <c r="C41" t="s">
+        <v>326</v>
+      </c>
+      <c r="D41" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="E41" t="s">
+        <v>235</v>
+      </c>
+      <c r="F41" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>185</v>
+      </c>
+      <c r="C42" t="s">
+        <v>329</v>
+      </c>
+      <c r="D42" t="s">
+        <v>258</v>
+      </c>
+      <c r="E42" t="s">
         <v>114</v>
       </c>
-      <c r="B21" t="s">
+      <c r="F42" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>184</v>
+      </c>
+      <c r="C43" t="s">
+        <v>281</v>
+      </c>
+      <c r="D43" t="s">
+        <v>245</v>
+      </c>
+      <c r="E43" t="s">
+        <v>327</v>
+      </c>
+      <c r="F43" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>183</v>
+      </c>
+      <c r="C44" t="s">
         <v>116</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D44" t="s">
+        <v>297</v>
+      </c>
+      <c r="E44" t="s">
+        <v>335</v>
+      </c>
+      <c r="F44" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>182</v>
+      </c>
+      <c r="C45" t="s">
+        <v>269</v>
+      </c>
+      <c r="D45" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="E45" t="s">
+        <v>253</v>
+      </c>
+      <c r="F45" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>181</v>
+      </c>
+      <c r="C46" t="s">
+        <v>319</v>
+      </c>
+      <c r="D46" t="s">
+        <v>301</v>
+      </c>
+      <c r="E46" t="s">
         <v>118</v>
       </c>
-      <c r="B23" t="s">
+      <c r="F46" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
+        <v>180</v>
+      </c>
+      <c r="C47" t="s">
+        <v>255</v>
+      </c>
+      <c r="D47" t="s">
+        <v>231</v>
+      </c>
+      <c r="E47" t="s">
+        <v>244</v>
+      </c>
+      <c r="F47" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>179</v>
+      </c>
+      <c r="C48" t="s">
         <v>120</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D48" t="s">
+        <v>231</v>
+      </c>
+      <c r="E48" t="s">
+        <v>271</v>
+      </c>
+      <c r="F48" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
+        <v>178</v>
+      </c>
+      <c r="C49" t="s">
+        <v>232</v>
+      </c>
+      <c r="D49" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="E49" t="s">
+        <v>259</v>
+      </c>
+      <c r="F49" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50" t="s">
+        <v>177</v>
+      </c>
+      <c r="C50" t="s">
+        <v>329</v>
+      </c>
+      <c r="D50" t="s">
+        <v>337</v>
+      </c>
+      <c r="E50" t="s">
         <v>122</v>
       </c>
-      <c r="B25" t="s">
+      <c r="F50" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>176</v>
+      </c>
+      <c r="C51" t="s">
+        <v>339</v>
+      </c>
+      <c r="D51" t="s">
+        <v>340</v>
+      </c>
+      <c r="E51" t="s">
+        <v>195</v>
+      </c>
+      <c r="F51" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>175</v>
+      </c>
+      <c r="C52" t="s">
         <v>124</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D52" t="s">
+        <v>334</v>
+      </c>
+      <c r="E52" t="s">
+        <v>329</v>
+      </c>
+      <c r="F52" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>174</v>
+      </c>
+      <c r="C53" t="s">
+        <v>214</v>
+      </c>
+      <c r="D53" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="E53" t="s">
+        <v>274</v>
+      </c>
+      <c r="F53" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>173</v>
+      </c>
+      <c r="C54" t="s">
+        <v>318</v>
+      </c>
+      <c r="D54" t="s">
+        <v>321</v>
+      </c>
+      <c r="E54" t="s">
         <v>126</v>
       </c>
-      <c r="B27" t="s">
+      <c r="F54" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>55</v>
+      </c>
+      <c r="B55" t="s">
+        <v>172</v>
+      </c>
+      <c r="C55" t="s">
+        <v>288</v>
+      </c>
+      <c r="D55" t="s">
+        <v>267</v>
+      </c>
+      <c r="E55" t="s">
+        <v>339</v>
+      </c>
+      <c r="F55" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56" t="s">
+        <v>171</v>
+      </c>
+      <c r="C56" t="s">
         <v>128</v>
       </c>
-      <c r="B28" t="s">
+      <c r="D56" t="s">
+        <v>319</v>
+      </c>
+      <c r="E56" t="s">
+        <v>295</v>
+      </c>
+      <c r="F56" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57" t="s">
+        <v>170</v>
+      </c>
+      <c r="C57" t="s">
+        <v>195</v>
+      </c>
+      <c r="D57" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="E57" t="s">
+        <v>320</v>
+      </c>
+      <c r="F57" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
+        <v>169</v>
+      </c>
+      <c r="C58" t="s">
+        <v>331</v>
+      </c>
+      <c r="D58" t="s">
+        <v>312</v>
+      </c>
+      <c r="E58" t="s">
         <v>130</v>
       </c>
-      <c r="B29" t="s">
+      <c r="F58" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
+        <v>168</v>
+      </c>
+      <c r="C59" t="s">
+        <v>296</v>
+      </c>
+      <c r="D59" t="s">
+        <v>286</v>
+      </c>
+      <c r="E59" t="s">
+        <v>205</v>
+      </c>
+      <c r="F59" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>167</v>
+      </c>
+      <c r="C60" t="s">
         <v>132</v>
       </c>
-      <c r="B30" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>134</v>
-      </c>
-      <c r="B31" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>136</v>
-      </c>
-      <c r="B32" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>138</v>
-      </c>
-      <c r="B33" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>140</v>
-      </c>
-      <c r="B34" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>142</v>
-      </c>
-      <c r="B35" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>144</v>
-      </c>
-      <c r="B36" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>146</v>
-      </c>
-      <c r="B37" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>148</v>
-      </c>
-      <c r="B38" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>150</v>
-      </c>
-      <c r="B39" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>152</v>
-      </c>
-      <c r="B40" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>154</v>
-      </c>
-      <c r="B41" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>156</v>
-      </c>
-      <c r="B42" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>158</v>
-      </c>
-      <c r="B43" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>160</v>
-      </c>
-      <c r="B44" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>162</v>
-      </c>
-      <c r="B45" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>164</v>
-      </c>
-      <c r="B46" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>166</v>
-      </c>
-      <c r="B47" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>168</v>
-      </c>
-      <c r="B48" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>171</v>
-      </c>
-      <c r="B49" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>172</v>
-      </c>
-      <c r="B50" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>174</v>
-      </c>
-      <c r="B51" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>176</v>
-      </c>
-      <c r="B52" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>178</v>
-      </c>
-      <c r="B53" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>180</v>
-      </c>
-      <c r="B54" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>182</v>
-      </c>
-      <c r="B55" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>184</v>
-      </c>
-      <c r="B56" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>186</v>
-      </c>
-      <c r="B57" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>188</v>
-      </c>
-      <c r="B58" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>190</v>
-      </c>
-      <c r="B59" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>192</v>
-      </c>
-      <c r="B60" t="s">
-        <v>193</v>
+      <c r="D60" t="s">
+        <v>249</v>
+      </c>
+      <c r="E60" t="s">
+        <v>312</v>
+      </c>
+      <c r="F60" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D148"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="61.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.6328125" customWidth="1"/>
+    <col min="5" max="5" width="38.36328125" customWidth="1"/>
+    <col min="6" max="6" width="39.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1">
+        <f ca="1">RANDBETWEEN(1,148)</f>
+        <v>141</v>
+      </c>
+      <c r="D1" t="str">
+        <f ca="1">LOOKUP($C1,A$1:A$148,B$1:B$148)</f>
+        <v>Acertar</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C65" ca="1" si="0">RANDBETWEEN(1,148)</f>
+        <v>4</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D65" ca="1" si="1">LOOKUP($C2,A$1:A$148,B$1:B$148)</f>
+        <v>Hasta luego.</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ca="1" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Ser un gallina</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ca="1" si="0"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ca="1" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ca="1" si="0"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>205</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ca="1" si="0"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>206</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>207</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ca="1" si="0"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>209</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ca="1" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>210</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ca="1" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>211</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>212</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ca="1" si="0"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>213</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ca="1" si="0"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>214</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ca="1" si="0"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>215</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ca="1" si="0"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>216</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ca="1" si="0"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>217</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ca="1" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>218</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>219</v>
+      </c>
+      <c r="C27">
+        <f t="shared" ca="1" si="0"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>220</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ca="1" si="0"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>221</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ca="1" si="0"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>222</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ca="1" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>223</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ca="1" si="0"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>224</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ca="1" si="0"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>225</v>
+      </c>
+      <c r="C33">
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>226</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ca="1" si="0"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>227</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ca="1" si="0"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>228</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>229</v>
+      </c>
+      <c r="C37">
+        <f t="shared" ca="1" si="0"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>230</v>
+      </c>
+      <c r="C38">
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>231</v>
+      </c>
+      <c r="C39">
+        <f t="shared" ca="1" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>232</v>
+      </c>
+      <c r="C40">
+        <f t="shared" ca="1" si="0"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>233</v>
+      </c>
+      <c r="C41">
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>234</v>
+      </c>
+      <c r="C42">
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>235</v>
+      </c>
+      <c r="C43">
+        <f t="shared" ca="1" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>236</v>
+      </c>
+      <c r="C44">
+        <f t="shared" ca="1" si="0"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>237</v>
+      </c>
+      <c r="C45">
+        <f t="shared" ca="1" si="0"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>238</v>
+      </c>
+      <c r="C46">
+        <f t="shared" ca="1" si="0"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
+        <v>239</v>
+      </c>
+      <c r="C47">
+        <f t="shared" ca="1" si="0"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>240</v>
+      </c>
+      <c r="C48">
+        <f t="shared" ca="1" si="0"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
+        <v>241</v>
+      </c>
+      <c r="C49">
+        <f t="shared" ca="1" si="0"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50" t="s">
+        <v>242</v>
+      </c>
+      <c r="C50">
+        <f t="shared" ca="1" si="0"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>243</v>
+      </c>
+      <c r="C51">
+        <f t="shared" ca="1" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>244</v>
+      </c>
+      <c r="C52">
+        <f t="shared" ca="1" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>245</v>
+      </c>
+      <c r="C53">
+        <f t="shared" ca="1" si="0"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>246</v>
+      </c>
+      <c r="C54">
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>55</v>
+      </c>
+      <c r="B55" t="s">
+        <v>247</v>
+      </c>
+      <c r="C55">
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56" t="s">
+        <v>248</v>
+      </c>
+      <c r="C56">
+        <f t="shared" ca="1" si="0"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57" t="s">
+        <v>249</v>
+      </c>
+      <c r="C57">
+        <f t="shared" ca="1" si="0"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
+        <v>250</v>
+      </c>
+      <c r="C58">
+        <f t="shared" ca="1" si="0"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
+        <v>251</v>
+      </c>
+      <c r="C59">
+        <f t="shared" ca="1" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>252</v>
+      </c>
+      <c r="C60">
+        <f t="shared" ca="1" si="0"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>61</v>
+      </c>
+      <c r="B61" t="s">
+        <v>253</v>
+      </c>
+      <c r="C61">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>254</v>
+      </c>
+      <c r="C62">
+        <f t="shared" ca="1" si="0"/>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>63</v>
+      </c>
+      <c r="B63" t="s">
+        <v>255</v>
+      </c>
+      <c r="C63">
+        <f t="shared" ca="1" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>64</v>
+      </c>
+      <c r="B64" t="s">
+        <v>256</v>
+      </c>
+      <c r="C64">
+        <f t="shared" ca="1" si="0"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
+        <v>257</v>
+      </c>
+      <c r="C65">
+        <f t="shared" ca="1" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
+        <v>258</v>
+      </c>
+      <c r="C66">
+        <f t="shared" ref="C66:C129" ca="1" si="2">RANDBETWEEN(1,148)</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>67</v>
+      </c>
+      <c r="B67" t="s">
+        <v>259</v>
+      </c>
+      <c r="C67">
+        <f t="shared" ca="1" si="2"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
+        <v>260</v>
+      </c>
+      <c r="C68">
+        <f t="shared" ca="1" si="2"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>69</v>
+      </c>
+      <c r="B69" t="s">
+        <v>261</v>
+      </c>
+      <c r="C69">
+        <f t="shared" ca="1" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>70</v>
+      </c>
+      <c r="B70" t="s">
+        <v>262</v>
+      </c>
+      <c r="C70">
+        <f t="shared" ca="1" si="2"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>71</v>
+      </c>
+      <c r="B71" t="s">
+        <v>263</v>
+      </c>
+      <c r="C71">
+        <f t="shared" ca="1" si="2"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>72</v>
+      </c>
+      <c r="B72" t="s">
+        <v>264</v>
+      </c>
+      <c r="C72">
+        <f t="shared" ca="1" si="2"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>73</v>
+      </c>
+      <c r="B73" t="s">
+        <v>265</v>
+      </c>
+      <c r="C73">
+        <f t="shared" ca="1" si="2"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>74</v>
+      </c>
+      <c r="B74" t="s">
+        <v>266</v>
+      </c>
+      <c r="C74">
+        <f t="shared" ca="1" si="2"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>75</v>
+      </c>
+      <c r="B75" t="s">
+        <v>267</v>
+      </c>
+      <c r="C75">
+        <f t="shared" ca="1" si="2"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>76</v>
+      </c>
+      <c r="B76" t="s">
+        <v>268</v>
+      </c>
+      <c r="C76">
+        <f t="shared" ca="1" si="2"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>77</v>
+      </c>
+      <c r="B77" t="s">
+        <v>269</v>
+      </c>
+      <c r="C77">
+        <f t="shared" ca="1" si="2"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>78</v>
+      </c>
+      <c r="B78" t="s">
+        <v>270</v>
+      </c>
+      <c r="C78">
+        <f t="shared" ca="1" si="2"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>79</v>
+      </c>
+      <c r="B79" t="s">
+        <v>271</v>
+      </c>
+      <c r="C79">
+        <f t="shared" ca="1" si="2"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>80</v>
+      </c>
+      <c r="B80" t="s">
+        <v>272</v>
+      </c>
+      <c r="C80">
+        <f t="shared" ca="1" si="2"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>81</v>
+      </c>
+      <c r="B81" t="s">
+        <v>273</v>
+      </c>
+      <c r="C81">
+        <f t="shared" ca="1" si="2"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>82</v>
+      </c>
+      <c r="B82" t="s">
+        <v>274</v>
+      </c>
+      <c r="C82">
+        <f t="shared" ca="1" si="2"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>83</v>
+      </c>
+      <c r="B83" t="s">
+        <v>275</v>
+      </c>
+      <c r="C83">
+        <f t="shared" ca="1" si="2"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>84</v>
+      </c>
+      <c r="B84" t="s">
+        <v>276</v>
+      </c>
+      <c r="C84">
+        <f t="shared" ca="1" si="2"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>85</v>
+      </c>
+      <c r="B85" t="s">
+        <v>277</v>
+      </c>
+      <c r="C85">
+        <f t="shared" ca="1" si="2"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>278</v>
+      </c>
+      <c r="C86">
+        <f t="shared" ca="1" si="2"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>87</v>
+      </c>
+      <c r="B87" t="s">
+        <v>279</v>
+      </c>
+      <c r="C87">
+        <f t="shared" ca="1" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>88</v>
+      </c>
+      <c r="B88" t="s">
+        <v>280</v>
+      </c>
+      <c r="C88">
+        <f t="shared" ca="1" si="2"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>89</v>
+      </c>
+      <c r="B89" t="s">
+        <v>281</v>
+      </c>
+      <c r="C89">
+        <f t="shared" ca="1" si="2"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>90</v>
+      </c>
+      <c r="B90" t="s">
+        <v>283</v>
+      </c>
+      <c r="C90">
+        <f t="shared" ca="1" si="2"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>91</v>
+      </c>
+      <c r="B91" t="s">
+        <v>285</v>
+      </c>
+      <c r="C91">
+        <f t="shared" ca="1" si="2"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>92</v>
+      </c>
+      <c r="B92" t="s">
+        <v>287</v>
+      </c>
+      <c r="C92">
+        <f t="shared" ca="1" si="2"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>93</v>
+      </c>
+      <c r="B93" t="s">
+        <v>289</v>
+      </c>
+      <c r="C93">
+        <f t="shared" ca="1" si="2"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>94</v>
+      </c>
+      <c r="B94" t="s">
+        <v>291</v>
+      </c>
+      <c r="C94">
+        <f t="shared" ca="1" si="2"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>95</v>
+      </c>
+      <c r="B95" t="s">
+        <v>293</v>
+      </c>
+      <c r="C95">
+        <f t="shared" ca="1" si="2"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>96</v>
+      </c>
+      <c r="B96" t="s">
+        <v>295</v>
+      </c>
+      <c r="C96">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>97</v>
+      </c>
+      <c r="B97" t="s">
+        <v>297</v>
+      </c>
+      <c r="C97">
+        <f t="shared" ca="1" si="2"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>98</v>
+      </c>
+      <c r="B98" t="s">
+        <v>299</v>
+      </c>
+      <c r="C98">
+        <f t="shared" ca="1" si="2"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>99</v>
+      </c>
+      <c r="B99" t="s">
+        <v>301</v>
+      </c>
+      <c r="C99">
+        <f t="shared" ca="1" si="2"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>100</v>
+      </c>
+      <c r="B100" t="s">
+        <v>303</v>
+      </c>
+      <c r="C100">
+        <f t="shared" ca="1" si="2"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>101</v>
+      </c>
+      <c r="B101" t="s">
+        <v>305</v>
+      </c>
+      <c r="C101">
+        <f t="shared" ca="1" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>102</v>
+      </c>
+      <c r="B102" t="s">
+        <v>307</v>
+      </c>
+      <c r="C102">
+        <f t="shared" ca="1" si="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>103</v>
+      </c>
+      <c r="B103" t="s">
+        <v>309</v>
+      </c>
+      <c r="C103">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>104</v>
+      </c>
+      <c r="B104" t="s">
+        <v>311</v>
+      </c>
+      <c r="C104">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>105</v>
+      </c>
+      <c r="B105" t="s">
+        <v>313</v>
+      </c>
+      <c r="C105">
+        <f t="shared" ca="1" si="2"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>106</v>
+      </c>
+      <c r="B106" t="s">
+        <v>315</v>
+      </c>
+      <c r="C106">
+        <f t="shared" ca="1" si="2"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107">
+        <v>107</v>
+      </c>
+      <c r="B107" t="s">
+        <v>317</v>
+      </c>
+      <c r="C107">
+        <f t="shared" ca="1" si="2"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <v>108</v>
+      </c>
+      <c r="B108" t="s">
+        <v>319</v>
+      </c>
+      <c r="C108">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <v>109</v>
+      </c>
+      <c r="B109" t="s">
+        <v>321</v>
+      </c>
+      <c r="C109">
+        <f t="shared" ca="1" si="2"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <v>110</v>
+      </c>
+      <c r="B110" t="s">
+        <v>323</v>
+      </c>
+      <c r="C110">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>111</v>
+      </c>
+      <c r="B111" t="s">
+        <v>325</v>
+      </c>
+      <c r="C111">
+        <f t="shared" ca="1" si="2"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>112</v>
+      </c>
+      <c r="B112" t="s">
+        <v>327</v>
+      </c>
+      <c r="C112">
+        <f t="shared" ca="1" si="2"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A113">
+        <v>113</v>
+      </c>
+      <c r="B113" t="s">
+        <v>329</v>
+      </c>
+      <c r="C113">
+        <f t="shared" ca="1" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114">
+        <v>114</v>
+      </c>
+      <c r="B114" t="s">
+        <v>331</v>
+      </c>
+      <c r="C114">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <v>115</v>
+      </c>
+      <c r="B115" t="s">
+        <v>333</v>
+      </c>
+      <c r="C115">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>116</v>
+      </c>
+      <c r="B116" t="s">
+        <v>335</v>
+      </c>
+      <c r="C116">
+        <f t="shared" ca="1" si="2"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>117</v>
+      </c>
+      <c r="B117" t="s">
+        <v>337</v>
+      </c>
+      <c r="C117">
+        <f t="shared" ca="1" si="2"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <v>118</v>
+      </c>
+      <c r="B118" t="s">
+        <v>339</v>
+      </c>
+      <c r="C118">
+        <f t="shared" ca="1" si="2"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A119">
+        <v>119</v>
+      </c>
+      <c r="B119" t="s">
+        <v>282</v>
+      </c>
+      <c r="C119">
+        <f t="shared" ca="1" si="2"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A120">
+        <v>120</v>
+      </c>
+      <c r="B120" t="s">
+        <v>284</v>
+      </c>
+      <c r="C120">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A121">
+        <v>121</v>
+      </c>
+      <c r="B121" t="s">
+        <v>286</v>
+      </c>
+      <c r="C121">
+        <f t="shared" ca="1" si="2"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A122">
+        <v>122</v>
+      </c>
+      <c r="B122" t="s">
+        <v>288</v>
+      </c>
+      <c r="C122">
+        <f t="shared" ca="1" si="2"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A123">
+        <v>123</v>
+      </c>
+      <c r="B123" t="s">
+        <v>290</v>
+      </c>
+      <c r="C123">
+        <f t="shared" ca="1" si="2"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124">
+        <v>124</v>
+      </c>
+      <c r="B124" t="s">
+        <v>292</v>
+      </c>
+      <c r="C124">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A125">
+        <v>125</v>
+      </c>
+      <c r="B125" t="s">
+        <v>294</v>
+      </c>
+      <c r="C125">
+        <f t="shared" ca="1" si="2"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A126">
+        <v>126</v>
+      </c>
+      <c r="B126" t="s">
+        <v>296</v>
+      </c>
+      <c r="C126">
+        <f t="shared" ca="1" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A127">
+        <v>127</v>
+      </c>
+      <c r="B127" t="s">
+        <v>298</v>
+      </c>
+      <c r="C127">
+        <f t="shared" ca="1" si="2"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A128">
+        <v>128</v>
+      </c>
+      <c r="B128" t="s">
+        <v>300</v>
+      </c>
+      <c r="C128">
+        <f t="shared" ca="1" si="2"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129">
+        <v>129</v>
+      </c>
+      <c r="B129" t="s">
+        <v>302</v>
+      </c>
+      <c r="C129">
+        <f t="shared" ca="1" si="2"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130">
+        <v>130</v>
+      </c>
+      <c r="B130" t="s">
+        <v>304</v>
+      </c>
+      <c r="C130">
+        <f t="shared" ref="C130:C148" ca="1" si="3">RANDBETWEEN(1,148)</f>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A131">
+        <v>131</v>
+      </c>
+      <c r="B131" t="s">
+        <v>306</v>
+      </c>
+      <c r="C131">
+        <f t="shared" ca="1" si="3"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132">
+        <v>132</v>
+      </c>
+      <c r="B132" t="s">
+        <v>308</v>
+      </c>
+      <c r="C132">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133">
+        <v>133</v>
+      </c>
+      <c r="B133" t="s">
+        <v>310</v>
+      </c>
+      <c r="C133">
+        <f t="shared" ca="1" si="3"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134">
+        <v>134</v>
+      </c>
+      <c r="B134" t="s">
+        <v>312</v>
+      </c>
+      <c r="C134">
+        <f t="shared" ca="1" si="3"/>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135">
+        <v>135</v>
+      </c>
+      <c r="B135" t="s">
+        <v>314</v>
+      </c>
+      <c r="C135">
+        <f t="shared" ca="1" si="3"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136">
+        <v>136</v>
+      </c>
+      <c r="B136" t="s">
+        <v>316</v>
+      </c>
+      <c r="C136">
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137">
+        <v>137</v>
+      </c>
+      <c r="B137" t="s">
+        <v>318</v>
+      </c>
+      <c r="C137">
+        <f t="shared" ca="1" si="3"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138">
+        <v>138</v>
+      </c>
+      <c r="B138" t="s">
+        <v>320</v>
+      </c>
+      <c r="C138">
+        <f t="shared" ca="1" si="3"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139">
+        <v>139</v>
+      </c>
+      <c r="B139" t="s">
+        <v>322</v>
+      </c>
+      <c r="C139">
+        <f t="shared" ca="1" si="3"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140">
+        <v>140</v>
+      </c>
+      <c r="B140" t="s">
+        <v>324</v>
+      </c>
+      <c r="C140">
+        <f t="shared" ca="1" si="3"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141">
+        <v>141</v>
+      </c>
+      <c r="B141" t="s">
+        <v>326</v>
+      </c>
+      <c r="C141">
+        <f t="shared" ca="1" si="3"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142">
+        <v>142</v>
+      </c>
+      <c r="B142" t="s">
+        <v>328</v>
+      </c>
+      <c r="C142">
+        <f t="shared" ca="1" si="3"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143">
+        <v>143</v>
+      </c>
+      <c r="B143" t="s">
+        <v>330</v>
+      </c>
+      <c r="C143">
+        <f t="shared" ca="1" si="3"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144">
+        <v>144</v>
+      </c>
+      <c r="B144" t="s">
+        <v>332</v>
+      </c>
+      <c r="C144">
+        <f t="shared" ca="1" si="3"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145">
+        <v>145</v>
+      </c>
+      <c r="B145" t="s">
+        <v>334</v>
+      </c>
+      <c r="C145">
+        <f t="shared" ca="1" si="3"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146">
+        <v>146</v>
+      </c>
+      <c r="B146" t="s">
+        <v>336</v>
+      </c>
+      <c r="C146">
+        <f t="shared" ca="1" si="3"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A147">
+        <v>147</v>
+      </c>
+      <c r="B147" t="s">
+        <v>338</v>
+      </c>
+      <c r="C147">
+        <f t="shared" ca="1" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A148">
+        <v>148</v>
+      </c>
+      <c r="B148" t="s">
+        <v>340</v>
+      </c>
+      <c r="C148">
+        <f t="shared" ca="1" si="3"/>
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>